<commit_message>
Created a class to read the test from file
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,19 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\SauceDemo3rdGroup2025\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC438C9-DDE6-4484-9C8A-9D6CB05FC82F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,32 +18,9 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>standard_user</t>
-  </si>
-  <si>
-    <t>secrete_sauce</t>
-  </si>
-  <si>
-    <t>Sfisile</t>
-  </si>
-  <si>
-    <t>Mabuza</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,30 +28,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -88,29 +45,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,56 +330,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="20.77734375" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-    </row>
-  </sheetData>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>